<commit_message>
CR-782 Bom Export report modification
</commit_message>
<xml_diff>
--- a/App_Templates/BOM_Template.xlsx
+++ b/App_Templates/BOM_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Document</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -56,6 +53,18 @@
   </si>
   <si>
     <t>ITEM</t>
+  </si>
+  <si>
+    <t>SPOOL
+Weight</t>
+  </si>
+  <si>
+    <t>PART
+Weight</t>
+  </si>
+  <si>
+    <t>Drawing
+Weight</t>
   </si>
 </sst>
 </file>
@@ -132,34 +141,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,105 +489,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="6"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="7"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="6"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="J2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="N2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="Q2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CR-782 Updation required in Excel Report [Export Bom] from DMS-YAMUNANAGAR
</commit_message>
<xml_diff>
--- a/App_Templates/BOM_Template.xlsx
+++ b/App_Templates/BOM_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Document</t>
   </si>
@@ -65,13 +65,17 @@
   <si>
     <t>Drawing
 Weight</t>
+  </si>
+  <si>
+    <t>Spool
+Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +91,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -97,24 +109,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -137,11 +149,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,43 +198,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -489,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,102 +560,107 @@
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="4" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
     </row>
-    <row r="2" spans="1:18" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="M1:S1"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>